<commit_message>
solved issue: blank transformed std df due to not finding year column
</commit_message>
<xml_diff>
--- a/output/61bbdb19-1f94-4617-8814-9148f0a43000/61bbdb19-1f94-4617-8814-9148f0a43000_notes_cropped_df.xlsx
+++ b/output/61bbdb19-1f94-4617-8814-9148f0a43000/61bbdb19-1f94-4617-8814-9148f0a43000_notes_cropped_df.xlsx
@@ -7,28 +7,30 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="038f385a-1d6c-3f73-9" sheetId="1" r:id="rId1"/>
-    <sheet name="e49a50c5-fc40-348e-9" sheetId="2" r:id="rId2"/>
-    <sheet name="15014b4d-61d4-351c-a" sheetId="3" r:id="rId3"/>
-    <sheet name="c83758f9-d318-34d1-b" sheetId="4" r:id="rId4"/>
-    <sheet name="5c9b1d03-58f3-3784-9" sheetId="5" r:id="rId5"/>
-    <sheet name="51c61e95-fc3c-3ee3-b" sheetId="6" r:id="rId6"/>
-    <sheet name="ce85c201-f65d-3a89-b" sheetId="7" r:id="rId7"/>
-    <sheet name="ff944637-e0b0-3db1-8" sheetId="8" r:id="rId8"/>
-    <sheet name="d53d4967-c596-365d-8" sheetId="9" r:id="rId9"/>
-    <sheet name="ec79c015-ce95-34a0-b" sheetId="10" r:id="rId10"/>
-    <sheet name="0d429d65-e9d0-3dcd-8" sheetId="11" r:id="rId11"/>
-    <sheet name="ea17fabf-481c-3054-a" sheetId="12" r:id="rId12"/>
-    <sheet name="8ad934fd-533f-3a9b-a" sheetId="13" r:id="rId13"/>
-    <sheet name="e382c558-d8ea-313c-b" sheetId="14" r:id="rId14"/>
-    <sheet name="71b1f04c-7b10-3687-9" sheetId="15" r:id="rId15"/>
+    <sheet name="8__038f385a-1d6c-3f7" sheetId="1" r:id="rId1"/>
+    <sheet name="9__e49a50c5-fc40-348" sheetId="2" r:id="rId2"/>
+    <sheet name="10__15014b4d-61d4-35" sheetId="3" r:id="rId3"/>
+    <sheet name="7_(a)_c83758f9-d318-" sheetId="4" r:id="rId4"/>
+    <sheet name="7_(a)_5c9b1d03-58f3-" sheetId="5" r:id="rId5"/>
+    <sheet name="12__51c61e95-fc3c-3e" sheetId="6" r:id="rId6"/>
+    <sheet name="13__51c61e95-fc3c-3e" sheetId="7" r:id="rId7"/>
+    <sheet name="13__ce85c201-f65d-3a" sheetId="8" r:id="rId8"/>
+    <sheet name="14__ff944637-e0b0-3d" sheetId="9" r:id="rId9"/>
+    <sheet name="15__d53d4967-c596-36" sheetId="10" r:id="rId10"/>
+    <sheet name="15__ec79c015-ce95-34" sheetId="11" r:id="rId11"/>
+    <sheet name="15__0d429d65-e9d0-3d" sheetId="12" r:id="rId12"/>
+    <sheet name="15__ea17fabf-481c-30" sheetId="13" r:id="rId13"/>
+    <sheet name="16__c83758f9-d318-34" sheetId="14" r:id="rId14"/>
+    <sheet name="2__8ad934fd-533f-3a9" sheetId="15" r:id="rId15"/>
+    <sheet name="3__e382c558-d8ea-313" sheetId="16" r:id="rId16"/>
+    <sheet name="4__71b1f04c-7b10-368" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="178">
   <si>
     <t>8 Trade and other receivables</t>
   </si>
@@ -213,6 +215,297 @@
     <t>7514</t>
   </si>
   <si>
+    <t>Total recognised income and expense</t>
+  </si>
+  <si>
+    <t>Balance at 31 March</t>
+  </si>
+  <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
+    <t>On issue 1 April</t>
+  </si>
+  <si>
+    <t>On issue 31 March</t>
+  </si>
+  <si>
+    <t>17703</t>
+  </si>
+  <si>
+    <t>81732</t>
+  </si>
+  <si>
+    <t>Ordinary</t>
+  </si>
+  <si>
+    <t>Shares</t>
+  </si>
+  <si>
+    <t>'000</t>
+  </si>
+  <si>
+    <t>22400</t>
+  </si>
+  <si>
+    <t>10047</t>
+  </si>
+  <si>
+    <t>64029</t>
+  </si>
+  <si>
+    <t>Dividend franking account</t>
+  </si>
+  <si>
+    <t>Class C 30% (2021:30%) franking credits available to shareholders</t>
+  </si>
+  <si>
+    <t>ofthe Company for subsequent financial years</t>
+  </si>
+  <si>
+    <t>$'000</t>
+  </si>
+  <si>
+    <t>35875</t>
+  </si>
+  <si>
+    <t>31451</t>
+  </si>
+  <si>
+    <t>12 Trade and other payables</t>
+  </si>
+  <si>
+    <t>Trade payables due to parent entity Suzuki Motor Corporation</t>
+  </si>
+  <si>
+    <t>Other trade payables</t>
+  </si>
+  <si>
+    <t>Accrued expenses</t>
+  </si>
+  <si>
+    <t>Total trade and other payables</t>
+  </si>
+  <si>
+    <t>13 Employee benefits</t>
+  </si>
+  <si>
+    <t>18249</t>
+  </si>
+  <si>
+    <t>2419</t>
+  </si>
+  <si>
+    <t>16178</t>
+  </si>
+  <si>
+    <t>36847</t>
+  </si>
+  <si>
+    <t>18122</t>
+  </si>
+  <si>
+    <t>1451</t>
+  </si>
+  <si>
+    <t>14591</t>
+  </si>
+  <si>
+    <t>34164</t>
+  </si>
+  <si>
+    <t>2021 $000</t>
+  </si>
+  <si>
+    <t>Liability for annual and long- service leave</t>
+  </si>
+  <si>
+    <t>Non-current</t>
+  </si>
+  <si>
+    <t>Liability for long-service leave</t>
+  </si>
+  <si>
+    <t>2040</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>1850</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>Current leave obligations expected to be settled after 12</t>
+  </si>
+  <si>
+    <t>months</t>
+  </si>
+  <si>
+    <t>797</t>
+  </si>
+  <si>
+    <t>845</t>
+  </si>
+  <si>
+    <t>14 Provisions</t>
+  </si>
+  <si>
+    <t>Warranty</t>
+  </si>
+  <si>
+    <t>Payments made during the year</t>
+  </si>
+  <si>
+    <t>Provisions made during the year</t>
+  </si>
+  <si>
+    <t>4351</t>
+  </si>
+  <si>
+    <t>(961)</t>
+  </si>
+  <si>
+    <t>2279</t>
+  </si>
+  <si>
+    <t>5669</t>
+  </si>
+  <si>
+    <t>896</t>
+  </si>
+  <si>
+    <t>4773</t>
+  </si>
+  <si>
+    <t>2727</t>
+  </si>
+  <si>
+    <t>(746)</t>
+  </si>
+  <si>
+    <t>2370</t>
+  </si>
+  <si>
+    <t>1231</t>
+  </si>
+  <si>
+    <t>3120</t>
+  </si>
+  <si>
+    <t>Roadside assistance</t>
+  </si>
+  <si>
+    <t>4692</t>
+  </si>
+  <si>
+    <t>3796</t>
+  </si>
+  <si>
+    <t>15 Contract Liabilities</t>
+  </si>
+  <si>
+    <t>Retail Bonus adjustment</t>
+  </si>
+  <si>
+    <t>Dealer Holdback</t>
+  </si>
+  <si>
+    <t>Capped price service</t>
+  </si>
+  <si>
+    <t>Provisions (reversed)/made during the year</t>
+  </si>
+  <si>
+    <t>1330</t>
+  </si>
+  <si>
+    <t>2495</t>
+  </si>
+  <si>
+    <t>2731</t>
+  </si>
+  <si>
+    <t>(797)</t>
+  </si>
+  <si>
+    <t>(183)</t>
+  </si>
+  <si>
+    <t>1751</t>
+  </si>
+  <si>
+    <t>759</t>
+  </si>
+  <si>
+    <t>992</t>
+  </si>
+  <si>
+    <t>854</t>
+  </si>
+  <si>
+    <t>1622</t>
+  </si>
+  <si>
+    <t>4078</t>
+  </si>
+  <si>
+    <t>(1,053)</t>
+  </si>
+  <si>
+    <t>(294)</t>
+  </si>
+  <si>
+    <t>1414</t>
+  </si>
+  <si>
+    <t>1317</t>
+  </si>
+  <si>
+    <t>Dealer incentive, promotionaland. DSM budget</t>
+  </si>
+  <si>
+    <t>1497</t>
+  </si>
+  <si>
+    <t>989</t>
+  </si>
+  <si>
+    <t>15 Contract Liabilities (continued)</t>
+  </si>
+  <si>
+    <t>Deferred Revenue</t>
+  </si>
+  <si>
+    <t>Total Contract Liabilities</t>
+  </si>
+  <si>
+    <t>1320</t>
+  </si>
+  <si>
+    <t>7402</t>
+  </si>
+  <si>
+    <t>5684</t>
+  </si>
+  <si>
+    <t>13086</t>
+  </si>
+  <si>
+    <t>494</t>
+  </si>
+  <si>
+    <t>5373</t>
+  </si>
+  <si>
+    <t>5113</t>
+  </si>
+  <si>
+    <t>10486</t>
+  </si>
+  <si>
     <t>Reconciliation of movement in capital and reserves.</t>
   </si>
   <si>
@@ -222,262 +515,10 @@
     <t>Balance at 1 April</t>
   </si>
   <si>
-    <t>Balance at 31 March</t>
-  </si>
-  <si>
     <t>Retained profits</t>
   </si>
   <si>
-    <t>Total recognised income and expense</t>
-  </si>
-  <si>
-    <t>Share Capital</t>
-  </si>
-  <si>
-    <t>On issue 1 April</t>
-  </si>
-  <si>
-    <t>On issue 31 March</t>
-  </si>
-  <si>
-    <t>$'000</t>
-  </si>
-  <si>
-    <t>22400</t>
-  </si>
-  <si>
-    <t>64029</t>
-  </si>
-  <si>
-    <t>17703</t>
-  </si>
-  <si>
-    <t>81732</t>
-  </si>
-  <si>
-    <t>Ordinary</t>
-  </si>
-  <si>
-    <t>Shares</t>
-  </si>
-  <si>
-    <t>'000</t>
-  </si>
-  <si>
     <t>53982</t>
-  </si>
-  <si>
-    <t>10047</t>
-  </si>
-  <si>
-    <t>Dividend franking account</t>
-  </si>
-  <si>
-    <t>Class C 30% (2021:30%) franking credits available to shareholders</t>
-  </si>
-  <si>
-    <t>ofthe Company for subsequent financial years</t>
-  </si>
-  <si>
-    <t>35875</t>
-  </si>
-  <si>
-    <t>31451</t>
-  </si>
-  <si>
-    <t>13 Employee benefits</t>
-  </si>
-  <si>
-    <t>Liability for annual and long- service leave</t>
-  </si>
-  <si>
-    <t>Non-current</t>
-  </si>
-  <si>
-    <t>Liability for long-service leave</t>
-  </si>
-  <si>
-    <t>2040</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>2021 $000</t>
-  </si>
-  <si>
-    <t>1850</t>
-  </si>
-  <si>
-    <t>146</t>
-  </si>
-  <si>
-    <t>Current leave obligations expected to be settled after 12</t>
-  </si>
-  <si>
-    <t>months</t>
-  </si>
-  <si>
-    <t>797</t>
-  </si>
-  <si>
-    <t>845</t>
-  </si>
-  <si>
-    <t>14 Provisions</t>
-  </si>
-  <si>
-    <t>Warranty</t>
-  </si>
-  <si>
-    <t>Payments made during the year</t>
-  </si>
-  <si>
-    <t>Provisions made during the year</t>
-  </si>
-  <si>
-    <t>4351</t>
-  </si>
-  <si>
-    <t>(961)</t>
-  </si>
-  <si>
-    <t>2279</t>
-  </si>
-  <si>
-    <t>5669</t>
-  </si>
-  <si>
-    <t>896</t>
-  </si>
-  <si>
-    <t>4773</t>
-  </si>
-  <si>
-    <t>2727</t>
-  </si>
-  <si>
-    <t>(746)</t>
-  </si>
-  <si>
-    <t>2370</t>
-  </si>
-  <si>
-    <t>1231</t>
-  </si>
-  <si>
-    <t>3120</t>
-  </si>
-  <si>
-    <t>Roadside assistance</t>
-  </si>
-  <si>
-    <t>4692</t>
-  </si>
-  <si>
-    <t>3796</t>
-  </si>
-  <si>
-    <t>15 Contract Liabilities</t>
-  </si>
-  <si>
-    <t>Retail Bonus adjustment</t>
-  </si>
-  <si>
-    <t>Dealer Holdback</t>
-  </si>
-  <si>
-    <t>Capped price service</t>
-  </si>
-  <si>
-    <t>Provisions (reversed)/made during the year</t>
-  </si>
-  <si>
-    <t>1330</t>
-  </si>
-  <si>
-    <t>2495</t>
-  </si>
-  <si>
-    <t>2731</t>
-  </si>
-  <si>
-    <t>(797)</t>
-  </si>
-  <si>
-    <t>(183)</t>
-  </si>
-  <si>
-    <t>1751</t>
-  </si>
-  <si>
-    <t>759</t>
-  </si>
-  <si>
-    <t>992</t>
-  </si>
-  <si>
-    <t>854</t>
-  </si>
-  <si>
-    <t>1622</t>
-  </si>
-  <si>
-    <t>4078</t>
-  </si>
-  <si>
-    <t>(1,053)</t>
-  </si>
-  <si>
-    <t>(294)</t>
-  </si>
-  <si>
-    <t>1414</t>
-  </si>
-  <si>
-    <t>1317</t>
-  </si>
-  <si>
-    <t>Dealer incentive, promotionaland. DSM budget</t>
-  </si>
-  <si>
-    <t>1497</t>
-  </si>
-  <si>
-    <t>989</t>
-  </si>
-  <si>
-    <t>15 Contract Liabilities (continued)</t>
-  </si>
-  <si>
-    <t>Deferred Revenue</t>
-  </si>
-  <si>
-    <t>Total Contract Liabilities</t>
-  </si>
-  <si>
-    <t>1320</t>
-  </si>
-  <si>
-    <t>7402</t>
-  </si>
-  <si>
-    <t>5684</t>
-  </si>
-  <si>
-    <t>13086</t>
-  </si>
-  <si>
-    <t>494</t>
-  </si>
-  <si>
-    <t>5373</t>
-  </si>
-  <si>
-    <t>5113</t>
-  </si>
-  <si>
-    <t>10486</t>
   </si>
   <si>
     <t>- Revenue</t>
@@ -983,6 +1024,81 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1002,7 +1118,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1013,21 +1129,21 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1035,23 +1151,23 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1064,21 +1180,21 @@
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1086,23 +1202,23 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="B13" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1115,13 +1231,13 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1129,32 +1245,32 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1162,10 +1278,10 @@
         <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1173,29 +1289,29 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1203,7 +1319,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1232,21 +1348,21 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1254,23 +1370,23 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1278,7 +1394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1299,7 +1415,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1310,21 +1426,21 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1332,23 +1448,23 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1361,13 +1477,13 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1375,29 +1491,29 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1405,7 +1521,164 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1426,65 +1699,65 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1492,7 +1765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1537,7 +1810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1843,7 +2116,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1864,132 +2137,70 @@
       <c r="A2" t="s">
         <v>61</v>
       </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
       <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2019,7 +2230,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2030,26 +2241,26 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2058,6 +2269,117 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2084,15 +2406,15 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2102,45 +2424,45 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2148,7 +2470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2177,7 +2499,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -2188,13 +2510,13 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2202,7 +2524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -2223,18 +2545,18 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2242,32 +2564,32 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2275,10 +2597,10 @@
         <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2286,104 +2608,29 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>